<commit_message>
API Test Homework No2 (Nova Poshta + Allure)
</commit_message>
<xml_diff>
--- a/src/test/resources/data/issues.xlsx
+++ b/src/test/resources/data/issues.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>bug</t>
   </si>
@@ -28,30 +28,6 @@
   </si>
   <si>
     <t>Some Text</t>
-  </si>
-  <si>
-    <t>Excel Auto Title 2</t>
-  </si>
-  <si>
-    <t>Excel Auto Title 3</t>
-  </si>
-  <si>
-    <t>Excel Auto Title 4</t>
-  </si>
-  <si>
-    <t>Excel Auto Title 5</t>
-  </si>
-  <si>
-    <t>Excel Auto Title 6</t>
-  </si>
-  <si>
-    <t>Excel Auto Title 7</t>
-  </si>
-  <si>
-    <t>documentation</t>
-  </si>
-  <si>
-    <t>question</t>
   </si>
 </sst>
 </file>
@@ -369,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E7" sqref="A2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,7 +360,7 @@
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -395,87 +371,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>